<commit_message>
Generated also a basic sitemap
</commit_message>
<xml_diff>
--- a/Solinteg Modbus Registers.xlsx
+++ b/Solinteg Modbus Registers.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41ABC2A9-91FC-4B68-93D2-3BE0F6AAACC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED36B67E-22DB-491D-BA3D-458553DC5CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Working Mode" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Registers!$A$1:$P$259</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Registers!$A$1:$Q$259</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1970" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="330">
   <si>
     <t>Table</t>
   </si>
@@ -1047,12 +1047,48 @@
   <si>
     <t>none</t>
   </si>
+  <si>
+    <t>sitemap group</t>
+  </si>
+  <si>
+    <t>Infos</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Phase A</t>
+  </si>
+  <si>
+    <t>Phase B</t>
+  </si>
+  <si>
+    <t>Phase C</t>
+  </si>
+  <si>
+    <t>All Phases</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Config</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1088,12 +1124,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Cali "/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1146,7 +1176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1171,17 +1201,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1208,10 +1237,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1539,12 +1564,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:P259"/>
+  <dimension ref="A1:Q259"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L207" sqref="L207:L208"/>
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q149" sqref="Q149:Q152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1565,10 +1589,11 @@
     <col min="14" max="14" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.42578125" style="1"/>
+    <col min="17" max="17" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1614,8 +1639,11 @@
       <c r="P1" s="4" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1646,7 +1674,7 @@
       <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="19">
+      <c r="L2" s="16">
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
@@ -1655,8 +1683,11 @@
       <c r="P2" s="1" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1666,14 +1697,14 @@
       <c r="C3" s="1">
         <v>10001</v>
       </c>
-      <c r="L3" s="19">
+      <c r="L3" s="16">
         <v>1</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1683,14 +1714,14 @@
       <c r="C4" s="1">
         <v>10002</v>
       </c>
-      <c r="L4" s="19">
+      <c r="L4" s="16">
         <v>1</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1700,14 +1731,14 @@
       <c r="C5" s="1">
         <v>10003</v>
       </c>
-      <c r="L5" s="19">
+      <c r="L5" s="16">
         <v>1</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1717,14 +1748,14 @@
       <c r="C6" s="1">
         <v>10004</v>
       </c>
-      <c r="L6" s="19">
+      <c r="L6" s="16">
         <v>1</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1734,14 +1765,14 @@
       <c r="C7" s="1">
         <v>10005</v>
       </c>
-      <c r="L7" s="19">
+      <c r="L7" s="16">
         <v>1</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1751,14 +1782,14 @@
       <c r="C8" s="1">
         <v>10006</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="16">
         <v>1</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1768,14 +1799,14 @@
       <c r="C9" s="1">
         <v>10007</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="16">
         <v>1</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1806,14 +1837,17 @@
       <c r="J10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="19">
+      <c r="L10" s="16">
         <v>1</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="Q10" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1844,14 +1878,17 @@
       <c r="J11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="19">
+      <c r="L11" s="16">
         <v>1</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="Q11" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1882,11 +1919,11 @@
       <c r="J12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="L12" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1914,17 +1951,20 @@
       <c r="I13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="J13" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="L13" s="19">
+      <c r="L13" s="16">
         <v>1</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="Q13" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1952,15 +1992,18 @@
       <c r="I14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="16"/>
-      <c r="L14" s="19">
+      <c r="J14" s="18"/>
+      <c r="L14" s="16">
         <v>1</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="Q14" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1988,15 +2031,18 @@
       <c r="I15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="L15" s="19">
+      <c r="J15" s="18"/>
+      <c r="L15" s="16">
         <v>1</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" hidden="1">
+      <c r="Q15" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -2033,8 +2079,11 @@
       <c r="P16" s="1" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" ht="90" hidden="1" customHeight="1">
+      <c r="Q16" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="90" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -2071,8 +2120,11 @@
       <c r="P17" s="1" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="Q17" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
@@ -2100,10 +2152,10 @@
       <c r="I18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="16" t="s">
+      <c r="J18" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="16">
         <v>1</v>
       </c>
       <c r="M18" s="1" t="s">
@@ -2112,8 +2164,11 @@
       <c r="P18" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -2141,15 +2196,15 @@
       <c r="I19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J19" s="16"/>
-      <c r="L19" s="19">
+      <c r="J19" s="18"/>
+      <c r="L19" s="16">
         <v>1</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -2177,8 +2232,8 @@
       <c r="I20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J20" s="16"/>
-      <c r="L20" s="19">
+      <c r="J20" s="18"/>
+      <c r="L20" s="16">
         <v>1</v>
       </c>
       <c r="M20" s="1" t="s">
@@ -2187,8 +2242,11 @@
       <c r="P20" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="Q20" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -2216,15 +2274,15 @@
       <c r="I21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J21" s="16"/>
-      <c r="L21" s="19">
+      <c r="J21" s="18"/>
+      <c r="L21" s="16">
         <v>1</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -2252,8 +2310,8 @@
       <c r="I22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J22" s="16"/>
-      <c r="L22" s="19">
+      <c r="J22" s="18"/>
+      <c r="L22" s="16">
         <v>1</v>
       </c>
       <c r="M22" s="1" t="s">
@@ -2262,8 +2320,11 @@
       <c r="P22" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="Q22" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -2291,15 +2352,15 @@
       <c r="I23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J23" s="16"/>
-      <c r="L23" s="19">
+      <c r="J23" s="18"/>
+      <c r="L23" s="16">
         <v>1</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="24" spans="1:16" hidden="1">
+    <row r="24" spans="1:17">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -2327,12 +2388,15 @@
       <c r="I24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J24" s="16"/>
+      <c r="J24" s="18"/>
       <c r="P24" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" hidden="1">
+      <c r="Q24" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
@@ -2364,7 +2428,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:16" hidden="1">
+    <row r="26" spans="1:17">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
@@ -2398,8 +2462,11 @@
       <c r="P26" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" hidden="1">
+      <c r="Q26" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27" s="1" t="s">
         <v>11</v>
       </c>
@@ -2410,7 +2477,7 @@
         <v>10997</v>
       </c>
     </row>
-    <row r="28" spans="1:16" hidden="1">
+    <row r="28" spans="1:17">
       <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
@@ -2441,8 +2508,11 @@
       <c r="P28" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" hidden="1">
+      <c r="Q28" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
@@ -2474,7 +2544,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:16" hidden="1">
+    <row r="30" spans="1:17">
       <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
@@ -2508,8 +2578,11 @@
       <c r="P30" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" hidden="1">
+      <c r="Q30" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -2541,7 +2614,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:16" hidden="1">
+    <row r="32" spans="1:17">
       <c r="A32" s="1" t="s">
         <v>11</v>
       </c>
@@ -2572,8 +2645,11 @@
       <c r="P32" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" hidden="1">
+      <c r="Q32" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
@@ -2605,7 +2681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:16" hidden="1">
+    <row r="34" spans="1:17">
       <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
@@ -2639,8 +2715,11 @@
       <c r="P34" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" hidden="1">
+      <c r="Q34" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35" s="1" t="s">
         <v>11</v>
       </c>
@@ -2672,7 +2751,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:16" hidden="1">
+    <row r="36" spans="1:17">
       <c r="A36" s="1" t="s">
         <v>11</v>
       </c>
@@ -2706,8 +2785,11 @@
       <c r="P36" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" hidden="1">
+      <c r="Q36" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37" s="1" t="s">
         <v>11</v>
       </c>
@@ -2741,8 +2823,11 @@
       <c r="P37" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" hidden="1">
+      <c r="Q37" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38" s="1" t="s">
         <v>11</v>
       </c>
@@ -2776,8 +2861,11 @@
       <c r="P38" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" hidden="1">
+      <c r="Q38" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39" s="1" t="s">
         <v>11</v>
       </c>
@@ -2811,8 +2899,11 @@
       <c r="P39" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" hidden="1">
+      <c r="Q39" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
       <c r="A40" s="1" t="s">
         <v>11</v>
       </c>
@@ -2846,8 +2937,11 @@
       <c r="P40" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" hidden="1">
+      <c r="Q40" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
       <c r="A41" s="1" t="s">
         <v>11</v>
       </c>
@@ -2881,8 +2975,11 @@
       <c r="P41" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" hidden="1">
+      <c r="Q41" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
       <c r="A42" s="1" t="s">
         <v>11</v>
       </c>
@@ -2916,8 +3013,11 @@
       <c r="P42" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" hidden="1">
+      <c r="Q42" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
       <c r="A43" s="1" t="s">
         <v>11</v>
       </c>
@@ -2951,8 +3051,11 @@
       <c r="P43" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" hidden="1">
+      <c r="Q43" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
       <c r="A44" s="1" t="s">
         <v>11</v>
       </c>
@@ -2986,8 +3089,11 @@
       <c r="P44" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" hidden="1">
+      <c r="Q44" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
       <c r="A45" s="1" t="s">
         <v>11</v>
       </c>
@@ -3021,8 +3127,11 @@
       <c r="P45" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" hidden="1">
+      <c r="Q45" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
       <c r="A46" s="1" t="s">
         <v>11</v>
       </c>
@@ -3056,8 +3165,11 @@
       <c r="P46" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" hidden="1">
+      <c r="Q46" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
@@ -3089,7 +3201,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:16" hidden="1">
+    <row r="48" spans="1:17">
       <c r="A48" s="1" t="s">
         <v>11</v>
       </c>
@@ -3123,8 +3235,11 @@
       <c r="P48" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" hidden="1">
+      <c r="Q48" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
       <c r="A49" s="1" t="s">
         <v>11</v>
       </c>
@@ -3156,7 +3271,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:16" hidden="1">
+    <row r="50" spans="1:17">
       <c r="A50" s="1" t="s">
         <v>11</v>
       </c>
@@ -3190,8 +3305,11 @@
       <c r="P50" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" hidden="1">
+      <c r="Q50" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17">
       <c r="A51" s="1" t="s">
         <v>11</v>
       </c>
@@ -3223,7 +3341,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:16" hidden="1">
+    <row r="52" spans="1:17">
       <c r="A52" s="1" t="s">
         <v>11</v>
       </c>
@@ -3254,8 +3372,11 @@
       <c r="P52" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" hidden="1">
+      <c r="Q52" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
       <c r="A53" s="1" t="s">
         <v>11</v>
       </c>
@@ -3287,7 +3408,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:16" hidden="1">
+    <row r="54" spans="1:17">
       <c r="A54" s="1" t="s">
         <v>11</v>
       </c>
@@ -3318,8 +3439,11 @@
       <c r="P54" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" hidden="1">
+      <c r="Q54" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17">
       <c r="A55" s="1" t="s">
         <v>11</v>
       </c>
@@ -3351,7 +3475,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:16" hidden="1">
+    <row r="56" spans="1:17">
       <c r="A56" s="1" t="s">
         <v>11</v>
       </c>
@@ -3385,8 +3509,11 @@
       <c r="P56" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" hidden="1">
+      <c r="Q56" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
       <c r="A57" s="1" t="s">
         <v>11</v>
       </c>
@@ -3420,8 +3547,11 @@
       <c r="P57" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="58" spans="1:16" hidden="1">
+      <c r="Q57" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17">
       <c r="A58" s="1" t="s">
         <v>11</v>
       </c>
@@ -3455,8 +3585,11 @@
       <c r="P58" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" hidden="1">
+      <c r="Q58" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17">
       <c r="A59" s="1" t="s">
         <v>11</v>
       </c>
@@ -3490,8 +3623,11 @@
       <c r="P59" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" hidden="1">
+      <c r="Q59" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17">
       <c r="A60" s="1" t="s">
         <v>11</v>
       </c>
@@ -3525,8 +3661,11 @@
       <c r="P60" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" hidden="1">
+      <c r="Q60" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17">
       <c r="A61" s="1" t="s">
         <v>11</v>
       </c>
@@ -3560,8 +3699,11 @@
       <c r="P61" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" hidden="1">
+      <c r="Q61" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17">
       <c r="A62" s="1" t="s">
         <v>11</v>
       </c>
@@ -3595,8 +3737,11 @@
       <c r="P62" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" hidden="1">
+      <c r="Q62" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17">
       <c r="A63" s="1" t="s">
         <v>11</v>
       </c>
@@ -3630,8 +3775,11 @@
       <c r="P63" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" hidden="1">
+      <c r="Q63" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
       <c r="A64" s="1" t="s">
         <v>11</v>
       </c>
@@ -3665,8 +3813,11 @@
       <c r="P64" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="65" spans="1:16" hidden="1">
+      <c r="Q64" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17">
       <c r="A65" s="1" t="s">
         <v>11</v>
       </c>
@@ -3698,7 +3849,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:16" hidden="1">
+    <row r="66" spans="1:17">
       <c r="A66" s="1" t="s">
         <v>11</v>
       </c>
@@ -3732,8 +3883,11 @@
       <c r="P66" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="67" spans="1:16" hidden="1">
+      <c r="Q66" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
       <c r="A67" s="1" t="s">
         <v>11</v>
       </c>
@@ -3765,7 +3919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:17">
       <c r="A68" s="1" t="s">
         <v>11</v>
       </c>
@@ -3793,10 +3947,10 @@
       <c r="I68" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J68" s="16" t="s">
+      <c r="J68" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="L68" s="19">
+      <c r="L68" s="16">
         <v>1</v>
       </c>
       <c r="M68" s="1" t="s">
@@ -3805,8 +3959,11 @@
       <c r="P68" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="69" spans="1:16">
+      <c r="Q68" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17">
       <c r="A69" s="1" t="s">
         <v>11</v>
       </c>
@@ -3834,15 +3991,15 @@
       <c r="I69" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J69" s="16"/>
-      <c r="L69" s="19">
+      <c r="J69" s="18"/>
+      <c r="L69" s="16">
         <v>1</v>
       </c>
       <c r="M69" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="70" spans="1:16" hidden="1">
+    <row r="70" spans="1:17">
       <c r="A70" s="1" t="s">
         <v>11</v>
       </c>
@@ -3876,8 +4033,11 @@
       <c r="P70" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="71" spans="1:16" hidden="1">
+      <c r="Q70" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17">
       <c r="A71" s="1" t="s">
         <v>11</v>
       </c>
@@ -3911,8 +4071,11 @@
       <c r="P71" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="72" spans="1:16" hidden="1">
+      <c r="Q71" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17">
       <c r="A72" s="1" t="s">
         <v>11</v>
       </c>
@@ -3946,8 +4109,11 @@
       <c r="P72" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="73" spans="1:16" hidden="1">
+      <c r="Q72" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17">
       <c r="A73" s="1" t="s">
         <v>11</v>
       </c>
@@ -3981,8 +4147,11 @@
       <c r="P73" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" hidden="1">
+      <c r="Q73" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17">
       <c r="A74" s="1" t="s">
         <v>11</v>
       </c>
@@ -4014,7 +4183,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:16" hidden="1">
+    <row r="75" spans="1:17">
       <c r="A75" s="1" t="s">
         <v>11</v>
       </c>
@@ -4048,8 +4217,11 @@
       <c r="P75" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" hidden="1">
+      <c r="Q75" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17">
       <c r="A76" s="1" t="s">
         <v>11</v>
       </c>
@@ -4083,8 +4255,11 @@
       <c r="P76" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="77" spans="1:16" hidden="1">
+      <c r="Q76" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17">
       <c r="A77" s="1" t="s">
         <v>11</v>
       </c>
@@ -4118,8 +4293,11 @@
       <c r="P77" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="78" spans="1:16" hidden="1">
+      <c r="Q77" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17">
       <c r="A78" s="1" t="s">
         <v>11</v>
       </c>
@@ -4153,8 +4331,11 @@
       <c r="P78" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="79" spans="1:16" hidden="1">
+      <c r="Q78" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17">
       <c r="A79" s="1" t="s">
         <v>11</v>
       </c>
@@ -4186,7 +4367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:16" hidden="1">
+    <row r="80" spans="1:17">
       <c r="A80" s="1" t="s">
         <v>11</v>
       </c>
@@ -4220,8 +4401,11 @@
       <c r="P80" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="81" spans="1:16" hidden="1">
+      <c r="Q80" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17">
       <c r="A81" s="1" t="s">
         <v>11</v>
       </c>
@@ -4255,8 +4439,11 @@
       <c r="P81" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="82" spans="1:16" hidden="1">
+      <c r="Q81" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17">
       <c r="A82" s="1" t="s">
         <v>11</v>
       </c>
@@ -4290,8 +4477,11 @@
       <c r="P82" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="83" spans="1:16" hidden="1">
+      <c r="Q82" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17">
       <c r="A83" s="1" t="s">
         <v>11</v>
       </c>
@@ -4325,8 +4515,11 @@
       <c r="P83" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="84" spans="1:16" hidden="1">
+      <c r="Q83" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17">
       <c r="A84" s="1" t="s">
         <v>11</v>
       </c>
@@ -4358,7 +4551,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:16" hidden="1">
+    <row r="85" spans="1:17">
       <c r="A85" s="1" t="s">
         <v>11</v>
       </c>
@@ -4392,8 +4585,11 @@
       <c r="P85" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="86" spans="1:16" hidden="1">
+      <c r="Q85" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17">
       <c r="A86" s="1" t="s">
         <v>11</v>
       </c>
@@ -4404,7 +4600,7 @@
         <v>20231</v>
       </c>
     </row>
-    <row r="87" spans="1:16" hidden="1">
+    <row r="87" spans="1:17">
       <c r="A87" s="1" t="s">
         <v>11</v>
       </c>
@@ -4438,8 +4634,11 @@
       <c r="P87" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="88" spans="1:16" hidden="1">
+      <c r="Q87" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17">
       <c r="A88" s="1" t="s">
         <v>11</v>
       </c>
@@ -4471,7 +4670,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:16" hidden="1">
+    <row r="89" spans="1:17">
       <c r="A89" s="1" t="s">
         <v>11</v>
       </c>
@@ -4505,8 +4704,11 @@
       <c r="P89" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="90" spans="1:16" hidden="1">
+      <c r="Q89" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17">
       <c r="A90" s="1" t="s">
         <v>11</v>
       </c>
@@ -4538,7 +4740,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:16" hidden="1">
+    <row r="91" spans="1:17">
       <c r="A91" s="1" t="s">
         <v>11</v>
       </c>
@@ -4572,8 +4774,11 @@
       <c r="P91" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="92" spans="1:16" hidden="1">
+      <c r="Q91" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17">
       <c r="A92" s="1" t="s">
         <v>11</v>
       </c>
@@ -4605,7 +4810,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:16" hidden="1">
+    <row r="93" spans="1:17">
       <c r="A93" s="1" t="s">
         <v>11</v>
       </c>
@@ -4639,8 +4844,11 @@
       <c r="P93" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="94" spans="1:16" hidden="1">
+      <c r="Q93" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17">
       <c r="A94" s="1" t="s">
         <v>11</v>
       </c>
@@ -4674,8 +4882,11 @@
       <c r="P94" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="95" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q94" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" ht="30" customHeight="1">
       <c r="A95" s="1" t="s">
         <v>11</v>
       </c>
@@ -4715,8 +4926,11 @@
       <c r="P95" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="96" spans="1:16" hidden="1">
+      <c r="Q95" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17">
       <c r="A96" s="1" t="s">
         <v>11</v>
       </c>
@@ -4750,8 +4964,11 @@
       <c r="P96" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="97" spans="1:16" hidden="1">
+      <c r="Q96" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17">
       <c r="A97" s="1" t="s">
         <v>11</v>
       </c>
@@ -4783,7 +5000,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:16" hidden="1">
+    <row r="98" spans="1:17">
       <c r="A98" s="1" t="s">
         <v>11</v>
       </c>
@@ -4814,8 +5031,11 @@
       <c r="P98" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="99" spans="1:16" hidden="1">
+      <c r="Q98" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17">
       <c r="A99" s="1" t="s">
         <v>11</v>
       </c>
@@ -4846,8 +5066,11 @@
       <c r="P99" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="100" spans="1:16" hidden="1">
+      <c r="Q99" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17">
       <c r="A100" s="1" t="s">
         <v>11</v>
       </c>
@@ -4878,8 +5101,11 @@
       <c r="P100" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="101" spans="1:16" hidden="1">
+      <c r="Q100" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17">
       <c r="A101" s="1" t="s">
         <v>11</v>
       </c>
@@ -4910,8 +5136,11 @@
       <c r="P101" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="102" spans="1:16" hidden="1">
+      <c r="Q101" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17">
       <c r="A102" s="1" t="s">
         <v>11</v>
       </c>
@@ -4942,8 +5171,11 @@
       <c r="P102" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="103" spans="1:16" hidden="1">
+      <c r="Q102" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17">
       <c r="A103" s="1" t="s">
         <v>11</v>
       </c>
@@ -4974,8 +5206,11 @@
       <c r="P103" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="104" spans="1:16" hidden="1">
+      <c r="Q103" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17">
       <c r="A104" s="1" t="s">
         <v>11</v>
       </c>
@@ -5006,8 +5241,11 @@
       <c r="P104" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="105" spans="1:16" hidden="1">
+      <c r="Q104" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17">
       <c r="A105" s="1" t="s">
         <v>11</v>
       </c>
@@ -5038,8 +5276,11 @@
       <c r="P105" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="106" spans="1:16" hidden="1">
+      <c r="Q105" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17">
       <c r="A106" s="1" t="s">
         <v>11</v>
       </c>
@@ -5070,8 +5311,11 @@
       <c r="P106" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="107" spans="1:16" hidden="1">
+      <c r="Q106" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17">
       <c r="A107" s="1" t="s">
         <v>11</v>
       </c>
@@ -5103,7 +5347,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:16" hidden="1">
+    <row r="108" spans="1:17">
       <c r="A108" s="1" t="s">
         <v>11</v>
       </c>
@@ -5134,8 +5378,11 @@
       <c r="P108" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="109" spans="1:16" hidden="1">
+      <c r="Q108" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17">
       <c r="A109" s="1" t="s">
         <v>11</v>
       </c>
@@ -5167,7 +5414,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:16" hidden="1">
+    <row r="110" spans="1:17">
       <c r="A110" s="1" t="s">
         <v>11</v>
       </c>
@@ -5198,8 +5445,11 @@
       <c r="P110" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="111" spans="1:16" hidden="1">
+      <c r="Q110" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17">
       <c r="A111" s="1" t="s">
         <v>11</v>
       </c>
@@ -5231,7 +5481,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:16" hidden="1">
+    <row r="112" spans="1:17">
       <c r="A112" s="1" t="s">
         <v>11</v>
       </c>
@@ -5262,8 +5512,11 @@
       <c r="P112" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="113" spans="1:16" hidden="1">
+      <c r="Q112" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17">
       <c r="A113" s="1" t="s">
         <v>11</v>
       </c>
@@ -5295,7 +5548,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:16" hidden="1">
+    <row r="114" spans="1:17">
       <c r="A114" s="1" t="s">
         <v>11</v>
       </c>
@@ -5326,8 +5579,11 @@
       <c r="P114" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="115" spans="1:16" hidden="1">
+      <c r="Q114" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17">
       <c r="A115" s="1" t="s">
         <v>11</v>
       </c>
@@ -5359,7 +5615,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="116" spans="1:16" hidden="1">
+    <row r="116" spans="1:17">
       <c r="A116" s="1" t="s">
         <v>11</v>
       </c>
@@ -5390,8 +5646,11 @@
       <c r="P116" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="117" spans="1:16" hidden="1">
+      <c r="Q116" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17">
       <c r="A117" s="1" t="s">
         <v>11</v>
       </c>
@@ -5423,7 +5682,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:16" hidden="1">
+    <row r="118" spans="1:17">
       <c r="A118" s="1" t="s">
         <v>11</v>
       </c>
@@ -5454,8 +5713,11 @@
       <c r="P118" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="119" spans="1:16" hidden="1">
+      <c r="Q118" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17">
       <c r="A119" s="1" t="s">
         <v>11</v>
       </c>
@@ -5487,7 +5749,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="1:16" hidden="1">
+    <row r="120" spans="1:17">
       <c r="A120" s="1" t="s">
         <v>11</v>
       </c>
@@ -5518,8 +5780,11 @@
       <c r="P120" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="121" spans="1:16" hidden="1">
+      <c r="Q120" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17">
       <c r="A121" s="1" t="s">
         <v>11</v>
       </c>
@@ -5551,7 +5816,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" spans="1:16" hidden="1">
+    <row r="122" spans="1:17">
       <c r="A122" s="1" t="s">
         <v>11</v>
       </c>
@@ -5582,8 +5847,11 @@
       <c r="P122" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="123" spans="1:16" hidden="1">
+      <c r="Q122" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17">
       <c r="A123" s="1" t="s">
         <v>11</v>
       </c>
@@ -5617,8 +5885,11 @@
       <c r="P123" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="124" spans="1:16" hidden="1">
+      <c r="Q123" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17">
       <c r="A124" s="1" t="s">
         <v>11</v>
       </c>
@@ -5652,8 +5923,11 @@
       <c r="P124" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="125" spans="1:16" hidden="1">
+      <c r="Q124" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17">
       <c r="A125" s="1" t="s">
         <v>11</v>
       </c>
@@ -5687,8 +5961,11 @@
       <c r="P125" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="126" spans="1:16" hidden="1">
+      <c r="Q125" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17">
       <c r="A126" s="1" t="s">
         <v>11</v>
       </c>
@@ -5722,8 +5999,11 @@
       <c r="P126" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="127" spans="1:16" hidden="1">
+      <c r="Q126" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17">
       <c r="A127" s="1" t="s">
         <v>11</v>
       </c>
@@ -5757,8 +6037,11 @@
       <c r="P127" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="128" spans="1:16" hidden="1">
+      <c r="Q127" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17">
       <c r="A128" s="1" t="s">
         <v>11</v>
       </c>
@@ -5789,8 +6072,11 @@
       <c r="P128" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="129" spans="1:16" hidden="1">
+      <c r="Q128" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17">
       <c r="A129" s="1" t="s">
         <v>11</v>
       </c>
@@ -5824,8 +6110,11 @@
       <c r="P129" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="130" spans="1:16" hidden="1">
+      <c r="Q129" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17">
       <c r="A130" s="1" t="s">
         <v>11</v>
       </c>
@@ -5859,8 +6148,11 @@
       <c r="P130" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="131" spans="1:16" hidden="1">
+      <c r="Q130" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17">
       <c r="A131" s="1" t="s">
         <v>11</v>
       </c>
@@ -5894,8 +6186,11 @@
       <c r="P131" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="132" spans="1:16" hidden="1">
+      <c r="Q131" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17">
       <c r="A132" s="1" t="s">
         <v>11</v>
       </c>
@@ -5926,8 +6221,11 @@
       <c r="P132" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="133" spans="1:16" hidden="1">
+      <c r="Q132" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17">
       <c r="A133" s="1" t="s">
         <v>11</v>
       </c>
@@ -5958,8 +6256,11 @@
       <c r="P133" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="134" spans="1:16" hidden="1">
+      <c r="Q133" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17">
       <c r="A134" s="1" t="s">
         <v>11</v>
       </c>
@@ -5990,8 +6291,11 @@
       <c r="P134" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="135" spans="1:16" hidden="1">
+      <c r="Q134" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17">
       <c r="A135" s="1" t="s">
         <v>11</v>
       </c>
@@ -6022,8 +6326,11 @@
       <c r="P135" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="136" spans="1:16" hidden="1">
+      <c r="Q135" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17">
       <c r="A136" s="1" t="s">
         <v>11</v>
       </c>
@@ -6054,8 +6361,11 @@
       <c r="P136" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="137" spans="1:16" hidden="1">
+      <c r="Q136" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17">
       <c r="A137" s="1" t="s">
         <v>11</v>
       </c>
@@ -6086,8 +6396,11 @@
       <c r="P137" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="138" spans="1:16" hidden="1">
+      <c r="Q137" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17">
       <c r="A138" s="1" t="s">
         <v>11</v>
       </c>
@@ -6121,8 +6434,11 @@
       <c r="P138" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="139" spans="1:16" hidden="1">
+      <c r="Q138" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17">
       <c r="A139" s="1" t="s">
         <v>11</v>
       </c>
@@ -6156,8 +6472,11 @@
       <c r="P139" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="140" spans="1:16" hidden="1">
+      <c r="Q139" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17">
       <c r="A140" s="1" t="s">
         <v>11</v>
       </c>
@@ -6191,8 +6510,11 @@
       <c r="P140" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="141" spans="1:16" hidden="1">
+      <c r="Q140" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17">
       <c r="A141" s="1" t="s">
         <v>11</v>
       </c>
@@ -6223,8 +6545,11 @@
       <c r="P141" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="142" spans="1:16" hidden="1">
+      <c r="Q141" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17">
       <c r="A142" s="1" t="s">
         <v>11</v>
       </c>
@@ -6238,7 +6563,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="143" spans="1:16" hidden="1">
+    <row r="143" spans="1:17">
       <c r="A143" s="1" t="s">
         <v>11</v>
       </c>
@@ -6269,8 +6594,11 @@
       <c r="P143" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="144" spans="1:16" hidden="1">
+      <c r="Q143" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17">
       <c r="A144" s="1" t="s">
         <v>11</v>
       </c>
@@ -6284,7 +6612,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="145" spans="1:16" hidden="1">
+    <row r="145" spans="1:17">
       <c r="A145" s="1" t="s">
         <v>11</v>
       </c>
@@ -6315,8 +6643,11 @@
       <c r="P145" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="146" spans="1:16" hidden="1">
+      <c r="Q145" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17">
       <c r="A146" s="1" t="s">
         <v>11</v>
       </c>
@@ -6347,8 +6678,11 @@
       <c r="P146" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="147" spans="1:16" hidden="1">
+      <c r="Q146" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17">
       <c r="A147" s="1" t="s">
         <v>11</v>
       </c>
@@ -6379,8 +6713,11 @@
       <c r="P147" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="148" spans="1:16" hidden="1">
+      <c r="Q147" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17">
       <c r="A148" s="1" t="s">
         <v>11</v>
       </c>
@@ -6411,8 +6748,11 @@
       <c r="P148" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="149" spans="1:16" ht="30" customHeight="1">
+      <c r="Q148" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" ht="30" customHeight="1">
       <c r="A149" s="1" t="s">
         <v>128</v>
       </c>
@@ -6425,13 +6765,13 @@
       <c r="D149" s="1">
         <v>1</v>
       </c>
-      <c r="E149" s="17" t="s">
+      <c r="E149" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="F149" s="16" t="s">
+      <c r="F149" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="G149" s="16" t="s">
+      <c r="G149" s="18" t="s">
         <v>19</v>
       </c>
       <c r="H149" s="1" t="s">
@@ -6443,14 +6783,17 @@
       <c r="J149" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="L149" s="19">
+      <c r="L149" s="16">
         <v>1</v>
       </c>
       <c r="P149" s="1" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="150" spans="1:16" ht="30" customHeight="1">
+      <c r="Q149" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="150" spans="1:17" ht="30" customHeight="1">
       <c r="A150" s="1" t="s">
         <v>128</v>
       </c>
@@ -6463,9 +6806,9 @@
       <c r="D150" s="1">
         <v>1</v>
       </c>
-      <c r="E150" s="17"/>
-      <c r="F150" s="16"/>
-      <c r="G150" s="16"/>
+      <c r="E150" s="19"/>
+      <c r="F150" s="18"/>
+      <c r="G150" s="18"/>
       <c r="H150" s="1" t="s">
         <v>15</v>
       </c>
@@ -6475,14 +6818,17 @@
       <c r="J150" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="L150" s="19">
+      <c r="L150" s="16">
         <v>1</v>
       </c>
       <c r="P150" s="1" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="151" spans="1:16" ht="30" customHeight="1">
+      <c r="Q150" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17" ht="30" customHeight="1">
       <c r="A151" s="1" t="s">
         <v>128</v>
       </c>
@@ -6495,9 +6841,9 @@
       <c r="D151" s="1">
         <v>1</v>
       </c>
-      <c r="E151" s="17"/>
-      <c r="F151" s="16"/>
-      <c r="G151" s="16"/>
+      <c r="E151" s="19"/>
+      <c r="F151" s="18"/>
+      <c r="G151" s="18"/>
       <c r="H151" s="1" t="s">
         <v>15</v>
       </c>
@@ -6507,14 +6853,17 @@
       <c r="J151" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="L151" s="19">
+      <c r="L151" s="16">
         <v>1</v>
       </c>
       <c r="P151" s="1" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="152" spans="1:16" hidden="1">
+      <c r="Q151" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="152" spans="1:17">
       <c r="A152" s="1" t="s">
         <v>128</v>
       </c>
@@ -6548,8 +6897,11 @@
       <c r="P152" s="1" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="153" spans="1:16" ht="45" hidden="1" customHeight="1">
+      <c r="Q152" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="153" spans="1:17" ht="45" customHeight="1">
       <c r="A153" s="1" t="s">
         <v>128</v>
       </c>
@@ -6586,8 +6938,11 @@
       <c r="P153" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="154" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q153" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17" ht="30" customHeight="1">
       <c r="A154" s="1" t="s">
         <v>128</v>
       </c>
@@ -6624,8 +6979,11 @@
       <c r="P154" s="1" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="155" spans="1:16" hidden="1">
+      <c r="Q154" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17">
       <c r="A155" s="1" t="s">
         <v>128</v>
       </c>
@@ -6659,8 +7017,11 @@
       <c r="P155" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="156" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q155" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17" ht="30" customHeight="1">
       <c r="A156" s="1" t="s">
         <v>128</v>
       </c>
@@ -6700,8 +7061,11 @@
       <c r="P156" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="157" spans="1:16" hidden="1">
+      <c r="Q156" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17">
       <c r="A157" s="1" t="s">
         <v>128</v>
       </c>
@@ -6735,8 +7099,11 @@
       <c r="P157" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="158" spans="1:16" hidden="1">
+      <c r="Q157" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17">
       <c r="A158" s="1" t="s">
         <v>128</v>
       </c>
@@ -6770,8 +7137,11 @@
       <c r="P158" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="159" spans="1:16" hidden="1">
+      <c r="Q158" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17">
       <c r="A159" s="1" t="s">
         <v>128</v>
       </c>
@@ -6805,8 +7175,11 @@
       <c r="P159" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="160" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q159" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17" ht="30" customHeight="1">
       <c r="A160" s="1" t="s">
         <v>128</v>
       </c>
@@ -6840,8 +7213,11 @@
       <c r="P160" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="161" spans="1:16" hidden="1">
+      <c r="Q160" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="161" spans="1:17">
       <c r="A161" s="1" t="s">
         <v>128</v>
       </c>
@@ -6875,8 +7251,11 @@
       <c r="P161" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="162" spans="1:16" ht="75" hidden="1" customHeight="1">
+      <c r="Q161" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="162" spans="1:17" ht="75" customHeight="1">
       <c r="A162" s="1" t="s">
         <v>128</v>
       </c>
@@ -6913,8 +7292,11 @@
       <c r="P162" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="163" spans="1:16" hidden="1">
+      <c r="Q162" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="163" spans="1:17">
       <c r="A163" s="1" t="s">
         <v>128</v>
       </c>
@@ -6948,8 +7330,11 @@
       <c r="P163" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="164" spans="1:16" hidden="1">
+      <c r="Q163" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="164" spans="1:17">
       <c r="A164" s="1" t="s">
         <v>128</v>
       </c>
@@ -6983,8 +7368,11 @@
       <c r="P164" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="165" spans="1:16" hidden="1">
+      <c r="Q164" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="165" spans="1:17">
       <c r="A165" s="1" t="s">
         <v>128</v>
       </c>
@@ -7018,8 +7406,11 @@
       <c r="P165" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="166" spans="1:16" hidden="1">
+      <c r="Q165" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="166" spans="1:17">
       <c r="A166" s="1" t="s">
         <v>128</v>
       </c>
@@ -7053,8 +7444,11 @@
       <c r="P166" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="167" spans="1:16" hidden="1">
+      <c r="Q166" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="167" spans="1:17">
       <c r="A167" s="1" t="s">
         <v>128</v>
       </c>
@@ -7088,8 +7482,11 @@
       <c r="P167" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="168" spans="1:16" hidden="1">
+      <c r="Q167" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="168" spans="1:17">
       <c r="A168" s="1" t="s">
         <v>128</v>
       </c>
@@ -7123,8 +7520,11 @@
       <c r="P168" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="169" spans="1:16" hidden="1">
+      <c r="Q168" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="169" spans="1:17">
       <c r="A169" s="1" t="s">
         <v>128</v>
       </c>
@@ -7158,8 +7558,11 @@
       <c r="P169" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="170" spans="1:16" hidden="1">
+      <c r="Q169" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="170" spans="1:17">
       <c r="A170" s="1" t="s">
         <v>128</v>
       </c>
@@ -7193,8 +7596,11 @@
       <c r="P170" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="171" spans="1:16" hidden="1">
+      <c r="Q170" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="171" spans="1:17">
       <c r="A171" s="1" t="s">
         <v>128</v>
       </c>
@@ -7228,8 +7634,11 @@
       <c r="P171" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="172" spans="1:16" hidden="1">
+      <c r="Q171" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="172" spans="1:17">
       <c r="A172" s="1" t="s">
         <v>128</v>
       </c>
@@ -7263,8 +7672,11 @@
       <c r="P172" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="173" spans="1:16" hidden="1">
+      <c r="Q172" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="173" spans="1:17">
       <c r="A173" s="1" t="s">
         <v>128</v>
       </c>
@@ -7298,8 +7710,11 @@
       <c r="P173" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="174" spans="1:16" hidden="1">
+      <c r="Q173" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="174" spans="1:17">
       <c r="A174" s="1" t="s">
         <v>128</v>
       </c>
@@ -7333,8 +7748,11 @@
       <c r="P174" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="175" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q174" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="175" spans="1:17" ht="30" customHeight="1">
       <c r="A175" s="1" t="s">
         <v>128</v>
       </c>
@@ -7371,8 +7789,11 @@
       <c r="P175" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="176" spans="1:16" hidden="1">
+      <c r="Q175" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="176" spans="1:17">
       <c r="A176" s="1" t="s">
         <v>128</v>
       </c>
@@ -7406,8 +7827,11 @@
       <c r="P176" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="177" spans="1:16" hidden="1">
+      <c r="Q176" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="177" spans="1:17">
       <c r="A177" s="1" t="s">
         <v>128</v>
       </c>
@@ -7444,8 +7868,11 @@
       <c r="P177" s="1" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="178" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q177" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="178" spans="1:17" ht="30" customHeight="1">
       <c r="A178" s="1" t="s">
         <v>128</v>
       </c>
@@ -7482,8 +7909,11 @@
       <c r="P178" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="179" spans="1:16" hidden="1">
+      <c r="Q178" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="179" spans="1:17">
       <c r="A179" s="1" t="s">
         <v>128</v>
       </c>
@@ -7514,8 +7944,11 @@
       <c r="P179" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="180" spans="1:16" hidden="1">
+      <c r="Q179" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="180" spans="1:17">
       <c r="A180" s="1" t="s">
         <v>128</v>
       </c>
@@ -7549,8 +7982,11 @@
       <c r="P180" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="181" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q180" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="181" spans="1:17" ht="30" customHeight="1">
       <c r="A181" s="1" t="s">
         <v>128</v>
       </c>
@@ -7587,8 +8023,11 @@
       <c r="P181" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="182" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q181" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="182" spans="1:17" ht="30" customHeight="1">
       <c r="A182" s="1" t="s">
         <v>128</v>
       </c>
@@ -7625,8 +8064,11 @@
       <c r="P182" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="183" spans="1:16" hidden="1">
+      <c r="Q182" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="183" spans="1:17">
       <c r="A183" s="1" t="s">
         <v>128</v>
       </c>
@@ -7657,8 +8099,11 @@
       <c r="P183" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="184" spans="1:16" ht="45" hidden="1" customHeight="1">
+      <c r="Q183" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="184" spans="1:17" ht="45" customHeight="1">
       <c r="A184" s="1" t="s">
         <v>128</v>
       </c>
@@ -7695,8 +8140,11 @@
       <c r="P184" s="1" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="185" spans="1:16" ht="75" hidden="1" customHeight="1">
+      <c r="Q184" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="185" spans="1:17" ht="75" customHeight="1">
       <c r="A185" s="1" t="s">
         <v>128</v>
       </c>
@@ -7733,8 +8181,11 @@
       <c r="P185" s="1" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="186" spans="1:16" hidden="1">
+      <c r="Q185" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="186" spans="1:17">
       <c r="A186" s="1" t="s">
         <v>128</v>
       </c>
@@ -7768,8 +8219,11 @@
       <c r="P186" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="187" spans="1:16" hidden="1">
+      <c r="Q186" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="187" spans="1:17">
       <c r="A187" s="1" t="s">
         <v>128</v>
       </c>
@@ -7803,8 +8257,11 @@
       <c r="P187" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="188" spans="1:16" hidden="1">
+      <c r="Q187" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="188" spans="1:17">
       <c r="A188" s="1" t="s">
         <v>128</v>
       </c>
@@ -7838,8 +8295,11 @@
       <c r="P188" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="189" spans="1:16" hidden="1">
+      <c r="Q188" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="189" spans="1:17">
       <c r="A189" s="1" t="s">
         <v>128</v>
       </c>
@@ -7873,8 +8333,11 @@
       <c r="P189" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="190" spans="1:16" hidden="1">
+      <c r="Q189" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="190" spans="1:17">
       <c r="A190" s="1" t="s">
         <v>128</v>
       </c>
@@ -7905,8 +8368,11 @@
       <c r="P190" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="191" spans="1:16" hidden="1">
+      <c r="Q190" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="191" spans="1:17">
       <c r="A191" s="1" t="s">
         <v>128</v>
       </c>
@@ -7937,8 +8403,11 @@
       <c r="P191" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="192" spans="1:16" hidden="1">
+      <c r="Q191" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="192" spans="1:17">
       <c r="A192" s="1" t="s">
         <v>128</v>
       </c>
@@ -7969,8 +8438,11 @@
       <c r="P192" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="193" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q192" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="193" spans="1:17" ht="30" customHeight="1">
       <c r="A193" s="1" t="s">
         <v>128</v>
       </c>
@@ -8010,8 +8482,11 @@
       <c r="P193" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="194" spans="1:16" hidden="1">
+      <c r="Q193" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="194" spans="1:17">
       <c r="A194" s="1" t="s">
         <v>128</v>
       </c>
@@ -8045,8 +8520,11 @@
       <c r="P194" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="195" spans="1:16" hidden="1">
+      <c r="Q194" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="195" spans="1:17">
       <c r="A195" s="1" t="s">
         <v>128</v>
       </c>
@@ -8083,8 +8561,11 @@
       <c r="P195" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="196" spans="1:16" hidden="1">
+      <c r="Q195" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="196" spans="1:17">
       <c r="A196" s="1" t="s">
         <v>128</v>
       </c>
@@ -8118,8 +8599,11 @@
       <c r="P196" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="197" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q196" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="197" spans="1:17" ht="30" customHeight="1">
       <c r="A197" s="1" t="s">
         <v>128</v>
       </c>
@@ -8156,8 +8640,11 @@
       <c r="P197" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="198" spans="1:16" hidden="1">
+      <c r="Q197" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="198" spans="1:17">
       <c r="A198" s="1" t="s">
         <v>128</v>
       </c>
@@ -8191,8 +8678,11 @@
       <c r="P198" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="199" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q198" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="199" spans="1:17" ht="30" customHeight="1">
       <c r="A199" s="1" t="s">
         <v>128</v>
       </c>
@@ -8229,8 +8719,11 @@
       <c r="P199" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="200" spans="1:16" hidden="1">
+      <c r="Q199" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="200" spans="1:17">
       <c r="A200" s="1" t="s">
         <v>128</v>
       </c>
@@ -8264,8 +8757,11 @@
       <c r="P200" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="201" spans="1:16" ht="60" customHeight="1">
+      <c r="Q200" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="201" spans="1:17" ht="60" customHeight="1">
       <c r="A201" s="1" t="s">
         <v>128</v>
       </c>
@@ -8296,7 +8792,7 @@
       <c r="J201" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="L201" s="19">
+      <c r="L201" s="16">
         <v>1</v>
       </c>
       <c r="M201" s="1" t="s">
@@ -8305,8 +8801,11 @@
       <c r="P201" s="1" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="202" spans="1:16" ht="45" hidden="1" customHeight="1">
+      <c r="Q201" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="202" spans="1:17" ht="45" customHeight="1">
       <c r="A202" s="1" t="s">
         <v>128</v>
       </c>
@@ -8340,8 +8839,11 @@
       <c r="P202" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="203" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q202" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="203" spans="1:17" ht="30" customHeight="1">
       <c r="A203" s="1" t="s">
         <v>128</v>
       </c>
@@ -8378,8 +8880,11 @@
       <c r="P203" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="204" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q203" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="204" spans="1:17" ht="30" customHeight="1">
       <c r="A204" s="1" t="s">
         <v>128</v>
       </c>
@@ -8416,8 +8921,11 @@
       <c r="P204" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="205" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q204" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="205" spans="1:17" ht="30" customHeight="1">
       <c r="A205" s="1" t="s">
         <v>128</v>
       </c>
@@ -8451,8 +8959,11 @@
       <c r="P205" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="206" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q205" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="206" spans="1:17" ht="30" customHeight="1">
       <c r="A206" s="1" t="s">
         <v>128</v>
       </c>
@@ -8489,8 +9000,11 @@
       <c r="P206" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="207" spans="1:16">
+      <c r="Q206" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="207" spans="1:17">
       <c r="A207" s="1" t="s">
         <v>128</v>
       </c>
@@ -8518,17 +9032,20 @@
       <c r="I207" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J207" s="18" t="s">
+      <c r="J207" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="L207" s="20">
+      <c r="L207" s="1">
         <v>1</v>
       </c>
       <c r="P207" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="208" spans="1:16">
+      <c r="Q207" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="208" spans="1:17">
       <c r="A208" s="1" t="s">
         <v>128</v>
       </c>
@@ -8556,15 +9073,18 @@
       <c r="I208" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J208" s="18"/>
-      <c r="L208" s="20">
+      <c r="J208" s="17"/>
+      <c r="L208" s="1">
         <v>1</v>
       </c>
       <c r="P208" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="209" spans="1:16" hidden="1">
+      <c r="Q208" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="209" spans="1:17">
       <c r="A209" s="1" t="s">
         <v>128</v>
       </c>
@@ -8592,14 +9112,17 @@
       <c r="I209" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J209" s="18" t="s">
+      <c r="J209" s="17" t="s">
         <v>217</v>
       </c>
       <c r="P209" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="210" spans="1:16" hidden="1">
+      <c r="Q209" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="210" spans="1:17">
       <c r="A210" s="1" t="s">
         <v>128</v>
       </c>
@@ -8627,15 +9150,18 @@
       <c r="I210" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J210" s="18"/>
+      <c r="J210" s="17"/>
       <c r="M210" s="1" t="s">
         <v>289</v>
       </c>
       <c r="P210" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="211" spans="1:16" hidden="1">
+      <c r="Q210" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="211" spans="1:17">
       <c r="A211" s="1" t="s">
         <v>128</v>
       </c>
@@ -8663,15 +9189,18 @@
       <c r="I211" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J211" s="18"/>
+      <c r="J211" s="17"/>
       <c r="O211" s="1">
         <v>1</v>
       </c>
       <c r="P211" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="212" spans="1:16" hidden="1">
+      <c r="Q211" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="212" spans="1:17">
       <c r="A212" s="1" t="s">
         <v>128</v>
       </c>
@@ -8699,12 +9228,15 @@
       <c r="I212" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J212" s="18"/>
+      <c r="J212" s="17"/>
       <c r="P212" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="213" spans="1:16" hidden="1">
+      <c r="Q212" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="213" spans="1:17">
       <c r="A213" s="1" t="s">
         <v>128</v>
       </c>
@@ -8732,15 +9264,18 @@
       <c r="I213" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J213" s="18"/>
+      <c r="J213" s="17"/>
       <c r="O213" s="1">
         <v>1</v>
       </c>
       <c r="P213" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="214" spans="1:16">
+      <c r="Q213" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="214" spans="1:17">
       <c r="A214" s="1" t="s">
         <v>128</v>
       </c>
@@ -8768,15 +9303,18 @@
       <c r="I214" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J214" s="18"/>
-      <c r="L214" s="20">
+      <c r="J214" s="17"/>
+      <c r="L214" s="1">
         <v>1</v>
       </c>
       <c r="P214" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="215" spans="1:16">
+      <c r="Q214" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="215" spans="1:17">
       <c r="A215" s="1" t="s">
         <v>128</v>
       </c>
@@ -8804,15 +9342,18 @@
       <c r="I215" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J215" s="18"/>
-      <c r="L215" s="20">
+      <c r="J215" s="17"/>
+      <c r="L215" s="1">
         <v>1</v>
       </c>
       <c r="P215" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="216" spans="1:16" hidden="1">
+      <c r="Q215" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="216" spans="1:17">
       <c r="A216" s="1" t="s">
         <v>128</v>
       </c>
@@ -8840,14 +9381,17 @@
       <c r="I216" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J216" s="18" t="s">
+      <c r="J216" s="17" t="s">
         <v>218</v>
       </c>
       <c r="P216" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="217" spans="1:16" hidden="1">
+      <c r="Q216" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="217" spans="1:17">
       <c r="A217" s="1" t="s">
         <v>128</v>
       </c>
@@ -8875,15 +9419,18 @@
       <c r="I217" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J217" s="18"/>
+      <c r="J217" s="17"/>
       <c r="M217" s="1" t="s">
         <v>289</v>
       </c>
       <c r="P217" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="218" spans="1:16" hidden="1">
+      <c r="Q217" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="218" spans="1:17">
       <c r="A218" s="1" t="s">
         <v>128</v>
       </c>
@@ -8911,15 +9458,18 @@
       <c r="I218" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J218" s="18"/>
+      <c r="J218" s="17"/>
       <c r="O218" s="1">
         <v>1</v>
       </c>
       <c r="P218" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="219" spans="1:16" hidden="1">
+      <c r="Q218" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="219" spans="1:17">
       <c r="A219" s="1" t="s">
         <v>128</v>
       </c>
@@ -8947,12 +9497,15 @@
       <c r="I219" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J219" s="18"/>
+      <c r="J219" s="17"/>
       <c r="P219" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="220" spans="1:16" hidden="1">
+      <c r="Q219" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="220" spans="1:17">
       <c r="A220" s="1" t="s">
         <v>128</v>
       </c>
@@ -8980,15 +9533,18 @@
       <c r="I220" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J220" s="18"/>
+      <c r="J220" s="17"/>
       <c r="O220" s="1">
         <v>1</v>
       </c>
       <c r="P220" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="221" spans="1:16">
+      <c r="Q220" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="221" spans="1:17">
       <c r="A221" s="1" t="s">
         <v>128</v>
       </c>
@@ -9016,15 +9572,18 @@
       <c r="I221" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J221" s="18"/>
-      <c r="L221" s="20">
+      <c r="J221" s="17"/>
+      <c r="L221" s="1">
         <v>1</v>
       </c>
       <c r="P221" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="222" spans="1:16">
+      <c r="Q221" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="222" spans="1:17">
       <c r="A222" s="1" t="s">
         <v>128</v>
       </c>
@@ -9052,15 +9611,18 @@
       <c r="I222" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J222" s="18"/>
-      <c r="L222" s="20">
+      <c r="J222" s="17"/>
+      <c r="L222" s="1">
         <v>1</v>
       </c>
       <c r="P222" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="223" spans="1:16" hidden="1">
+      <c r="Q222" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="223" spans="1:17">
       <c r="A223" s="1" t="s">
         <v>128</v>
       </c>
@@ -9088,14 +9650,17 @@
       <c r="I223" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J223" s="18" t="s">
+      <c r="J223" s="17" t="s">
         <v>219</v>
       </c>
       <c r="P223" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="224" spans="1:16" hidden="1">
+      <c r="Q223" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="224" spans="1:17">
       <c r="A224" s="1" t="s">
         <v>128</v>
       </c>
@@ -9123,15 +9688,18 @@
       <c r="I224" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J224" s="18"/>
+      <c r="J224" s="17"/>
       <c r="M224" s="1" t="s">
         <v>289</v>
       </c>
       <c r="P224" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="225" spans="1:16" hidden="1">
+      <c r="Q224" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="225" spans="1:17">
       <c r="A225" s="1" t="s">
         <v>128</v>
       </c>
@@ -9159,15 +9727,18 @@
       <c r="I225" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J225" s="18"/>
+      <c r="J225" s="17"/>
       <c r="O225" s="1">
         <v>1</v>
       </c>
       <c r="P225" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="226" spans="1:16" hidden="1">
+      <c r="Q225" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="226" spans="1:17">
       <c r="A226" s="1" t="s">
         <v>128</v>
       </c>
@@ -9195,12 +9766,15 @@
       <c r="I226" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J226" s="18"/>
+      <c r="J226" s="17"/>
       <c r="P226" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="227" spans="1:16" hidden="1">
+      <c r="Q226" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="227" spans="1:17">
       <c r="A227" s="1" t="s">
         <v>128</v>
       </c>
@@ -9228,15 +9802,18 @@
       <c r="I227" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J227" s="18"/>
+      <c r="J227" s="17"/>
       <c r="O227" s="1">
         <v>1</v>
       </c>
       <c r="P227" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="228" spans="1:16">
+      <c r="Q227" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="228" spans="1:17">
       <c r="A228" s="1" t="s">
         <v>128</v>
       </c>
@@ -9264,15 +9841,18 @@
       <c r="I228" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J228" s="18"/>
-      <c r="L228" s="20">
+      <c r="J228" s="17"/>
+      <c r="L228" s="1">
         <v>1</v>
       </c>
       <c r="P228" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="229" spans="1:16">
+      <c r="Q228" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="229" spans="1:17">
       <c r="A229" s="1" t="s">
         <v>128</v>
       </c>
@@ -9300,15 +9880,18 @@
       <c r="I229" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J229" s="18"/>
-      <c r="L229" s="20">
+      <c r="J229" s="17"/>
+      <c r="L229" s="1">
         <v>1</v>
       </c>
       <c r="P229" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="230" spans="1:16" hidden="1">
+      <c r="Q229" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="230" spans="1:17">
       <c r="A230" s="1" t="s">
         <v>128</v>
       </c>
@@ -9336,14 +9919,17 @@
       <c r="I230" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J230" s="18" t="s">
+      <c r="J230" s="17" t="s">
         <v>220</v>
       </c>
       <c r="P230" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="231" spans="1:16" hidden="1">
+      <c r="Q230" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="231" spans="1:17">
       <c r="A231" s="1" t="s">
         <v>128</v>
       </c>
@@ -9371,15 +9957,18 @@
       <c r="I231" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J231" s="18"/>
+      <c r="J231" s="17"/>
       <c r="M231" s="1" t="s">
         <v>289</v>
       </c>
       <c r="P231" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="232" spans="1:16" hidden="1">
+      <c r="Q231" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="232" spans="1:17">
       <c r="A232" s="1" t="s">
         <v>128</v>
       </c>
@@ -9407,15 +9996,18 @@
       <c r="I232" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J232" s="18"/>
+      <c r="J232" s="17"/>
       <c r="O232" s="1">
         <v>1</v>
       </c>
       <c r="P232" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="233" spans="1:16" hidden="1">
+      <c r="Q232" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="233" spans="1:17">
       <c r="A233" s="1" t="s">
         <v>128</v>
       </c>
@@ -9443,12 +10035,15 @@
       <c r="I233" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J233" s="18"/>
+      <c r="J233" s="17"/>
       <c r="P233" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="234" spans="1:16" hidden="1">
+      <c r="Q233" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="234" spans="1:17">
       <c r="A234" s="1" t="s">
         <v>128</v>
       </c>
@@ -9476,15 +10071,18 @@
       <c r="I234" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J234" s="18"/>
+      <c r="J234" s="17"/>
       <c r="O234" s="1">
         <v>1</v>
       </c>
       <c r="P234" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="235" spans="1:16">
+      <c r="Q234" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="235" spans="1:17">
       <c r="A235" s="1" t="s">
         <v>128</v>
       </c>
@@ -9512,15 +10110,18 @@
       <c r="I235" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J235" s="18"/>
-      <c r="L235" s="20">
+      <c r="J235" s="17"/>
+      <c r="L235" s="1">
         <v>1</v>
       </c>
       <c r="P235" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="236" spans="1:16">
+      <c r="Q235" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="236" spans="1:17">
       <c r="A236" s="1" t="s">
         <v>128</v>
       </c>
@@ -9548,15 +10149,18 @@
       <c r="I236" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J236" s="18"/>
-      <c r="L236" s="20">
+      <c r="J236" s="17"/>
+      <c r="L236" s="1">
         <v>1</v>
       </c>
       <c r="P236" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="237" spans="1:16" hidden="1">
+      <c r="Q236" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="237" spans="1:17">
       <c r="A237" s="1" t="s">
         <v>128</v>
       </c>
@@ -9584,14 +10188,17 @@
       <c r="I237" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J237" s="18" t="s">
+      <c r="J237" s="17" t="s">
         <v>221</v>
       </c>
       <c r="P237" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="238" spans="1:16" hidden="1">
+      <c r="Q237" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="238" spans="1:17">
       <c r="A238" s="1" t="s">
         <v>128</v>
       </c>
@@ -9619,15 +10226,18 @@
       <c r="I238" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J238" s="18"/>
+      <c r="J238" s="17"/>
       <c r="M238" s="1" t="s">
         <v>289</v>
       </c>
       <c r="P238" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="239" spans="1:16" hidden="1">
+      <c r="Q238" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="239" spans="1:17">
       <c r="A239" s="1" t="s">
         <v>128</v>
       </c>
@@ -9655,15 +10265,18 @@
       <c r="I239" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J239" s="18"/>
+      <c r="J239" s="17"/>
       <c r="O239" s="1">
         <v>1</v>
       </c>
       <c r="P239" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="240" spans="1:16" hidden="1">
+      <c r="Q239" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="240" spans="1:17">
       <c r="A240" s="1" t="s">
         <v>128</v>
       </c>
@@ -9691,12 +10304,15 @@
       <c r="I240" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J240" s="18"/>
+      <c r="J240" s="17"/>
       <c r="P240" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="241" spans="1:16" hidden="1">
+      <c r="Q240" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="241" spans="1:17">
       <c r="A241" s="1" t="s">
         <v>128</v>
       </c>
@@ -9724,15 +10340,18 @@
       <c r="I241" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J241" s="18"/>
+      <c r="J241" s="17"/>
       <c r="O241" s="1">
         <v>1</v>
       </c>
       <c r="P241" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="242" spans="1:16">
+      <c r="Q241" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="242" spans="1:17">
       <c r="A242" s="1" t="s">
         <v>128</v>
       </c>
@@ -9760,15 +10379,18 @@
       <c r="I242" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J242" s="18"/>
-      <c r="L242" s="20">
+      <c r="J242" s="17"/>
+      <c r="L242" s="1">
         <v>1</v>
       </c>
       <c r="P242" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="243" spans="1:16">
+      <c r="Q242" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="243" spans="1:17">
       <c r="A243" s="1" t="s">
         <v>128</v>
       </c>
@@ -9796,15 +10418,18 @@
       <c r="I243" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J243" s="18"/>
-      <c r="L243" s="20">
+      <c r="J243" s="17"/>
+      <c r="L243" s="1">
         <v>1</v>
       </c>
       <c r="P243" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="244" spans="1:16" hidden="1">
+      <c r="Q243" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="244" spans="1:17">
       <c r="A244" s="1" t="s">
         <v>128</v>
       </c>
@@ -9841,8 +10466,11 @@
       <c r="P244" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="245" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q244" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="245" spans="1:17" ht="30" customHeight="1">
       <c r="A245" s="1" t="s">
         <v>128</v>
       </c>
@@ -9879,8 +10507,11 @@
       <c r="P245" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="246" spans="1:16" hidden="1">
+      <c r="Q245" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="246" spans="1:17">
       <c r="A246" s="1" t="s">
         <v>128</v>
       </c>
@@ -9908,7 +10539,7 @@
       <c r="I246" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J246" s="18" t="s">
+      <c r="J246" s="17" t="s">
         <v>226</v>
       </c>
       <c r="O246" s="1">
@@ -9917,8 +10548,11 @@
       <c r="P246" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="247" spans="1:16" hidden="1">
+      <c r="Q246" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="247" spans="1:17">
       <c r="A247" s="1" t="s">
         <v>128</v>
       </c>
@@ -9946,15 +10580,18 @@
       <c r="I247" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J247" s="18"/>
+      <c r="J247" s="17"/>
       <c r="O247" s="1">
         <v>1</v>
       </c>
       <c r="P247" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="248" spans="1:16" hidden="1">
+      <c r="Q247" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="248" spans="1:17">
       <c r="A248" s="1" t="s">
         <v>128</v>
       </c>
@@ -9982,15 +10619,18 @@
       <c r="I248" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J248" s="18"/>
+      <c r="J248" s="17"/>
       <c r="O248" s="1">
         <v>1</v>
       </c>
       <c r="P248" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="249" spans="1:16" hidden="1">
+      <c r="Q248" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="249" spans="1:17">
       <c r="A249" s="1" t="s">
         <v>128</v>
       </c>
@@ -10018,7 +10658,7 @@
       <c r="I249" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J249" s="16" t="s">
+      <c r="J249" s="18" t="s">
         <v>223</v>
       </c>
       <c r="O249" s="1">
@@ -10027,8 +10667,11 @@
       <c r="P249" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="250" spans="1:16" hidden="1">
+      <c r="Q249" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="250" spans="1:17">
       <c r="A250" s="1" t="s">
         <v>128</v>
       </c>
@@ -10056,15 +10699,18 @@
       <c r="I250" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J250" s="16"/>
+      <c r="J250" s="18"/>
       <c r="O250" s="1">
         <v>1</v>
       </c>
       <c r="P250" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="251" spans="1:16" hidden="1">
+      <c r="Q250" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="251" spans="1:17">
       <c r="A251" s="1" t="s">
         <v>128</v>
       </c>
@@ -10092,7 +10738,7 @@
       <c r="I251" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J251" s="16" t="s">
+      <c r="J251" s="18" t="s">
         <v>223</v>
       </c>
       <c r="O251" s="1">
@@ -10101,8 +10747,11 @@
       <c r="P251" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="252" spans="1:16" hidden="1">
+      <c r="Q251" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="252" spans="1:17">
       <c r="A252" s="1" t="s">
         <v>128</v>
       </c>
@@ -10130,15 +10779,18 @@
       <c r="I252" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J252" s="16"/>
+      <c r="J252" s="18"/>
       <c r="O252" s="1">
         <v>1</v>
       </c>
       <c r="P252" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="253" spans="1:16" hidden="1">
+      <c r="Q252" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="253" spans="1:17">
       <c r="A253" s="1" t="s">
         <v>128</v>
       </c>
@@ -10166,15 +10818,18 @@
       <c r="I253" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J253" s="16"/>
+      <c r="J253" s="18"/>
       <c r="O253" s="1">
         <v>1</v>
       </c>
       <c r="P253" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="254" spans="1:16" hidden="1">
+      <c r="Q253" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="254" spans="1:17">
       <c r="A254" s="1" t="s">
         <v>128</v>
       </c>
@@ -10202,15 +10857,18 @@
       <c r="I254" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J254" s="16"/>
+      <c r="J254" s="18"/>
       <c r="O254" s="1">
         <v>1</v>
       </c>
       <c r="P254" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="255" spans="1:16" hidden="1">
+      <c r="Q254" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="255" spans="1:17">
       <c r="A255" s="1" t="s">
         <v>128</v>
       </c>
@@ -10238,15 +10896,18 @@
       <c r="I255" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J255" s="16"/>
+      <c r="J255" s="18"/>
       <c r="O255" s="1">
         <v>1</v>
       </c>
       <c r="P255" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="256" spans="1:16" hidden="1">
+      <c r="Q255" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="256" spans="1:17">
       <c r="A256" s="1" t="s">
         <v>128</v>
       </c>
@@ -10274,15 +10935,18 @@
       <c r="I256" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J256" s="16"/>
+      <c r="J256" s="18"/>
       <c r="O256" s="1">
         <v>1</v>
       </c>
       <c r="P256" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="257" spans="1:16" hidden="1">
+      <c r="Q256" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="257" spans="1:17">
       <c r="A257" s="1" t="s">
         <v>128</v>
       </c>
@@ -10310,15 +10974,18 @@
       <c r="I257" s="1">
         <v>10</v>
       </c>
-      <c r="J257" s="16"/>
+      <c r="J257" s="18"/>
       <c r="O257" s="1">
         <v>1</v>
       </c>
       <c r="P257" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="258" spans="1:16" ht="30" hidden="1" customHeight="1">
+      <c r="Q257" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="258" spans="1:17" ht="30" customHeight="1">
       <c r="A258" s="1" t="s">
         <v>239</v>
       </c>
@@ -10355,8 +11022,11 @@
       <c r="P258" s="1" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="259" spans="1:16" hidden="1">
+      <c r="Q258" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="259" spans="1:17">
       <c r="A259" s="1" t="s">
         <v>239</v>
       </c>
@@ -10393,16 +11063,19 @@
       <c r="P259" s="1" t="s">
         <v>315</v>
       </c>
+      <c r="Q259" s="1" t="s">
+        <v>329</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P259" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="11">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Q259" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="15">
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="J18:J24"/>
+    <mergeCell ref="J68:J69"/>
+    <mergeCell ref="E149:E151"/>
+    <mergeCell ref="F149:F151"/>
+    <mergeCell ref="G149:G151"/>
     <mergeCell ref="J237:J243"/>
     <mergeCell ref="J246:J248"/>
     <mergeCell ref="J249:J250"/>
@@ -10412,12 +11085,6 @@
     <mergeCell ref="J216:J222"/>
     <mergeCell ref="J223:J229"/>
     <mergeCell ref="J230:J236"/>
-    <mergeCell ref="J13:J15"/>
-    <mergeCell ref="J18:J24"/>
-    <mergeCell ref="J68:J69"/>
-    <mergeCell ref="E149:E151"/>
-    <mergeCell ref="F149:F151"/>
-    <mergeCell ref="G149:G151"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="0"/>

</xml_diff>

<commit_message>
Sitemap extended with manually defined items, improved documentation
</commit_message>
<xml_diff>
--- a/Solinteg Modbus Registers.xlsx
+++ b/Solinteg Modbus Registers.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED36B67E-22DB-491D-BA3D-458553DC5CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A3A14E-0343-4E7C-A98B-E67AC724370F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="2" r:id="rId1"/>
     <sheet name="Data Types" sheetId="5" r:id="rId2"/>
     <sheet name="Working Mode" sheetId="6" r:id="rId3"/>
+    <sheet name="Manual Config" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Registers!$A$1:$Q$259</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2317" uniqueCount="403">
   <si>
     <t>Table</t>
   </si>
@@ -1083,12 +1084,231 @@
   <si>
     <t>Control</t>
   </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>PV_Device_SN</t>
+  </si>
+  <si>
+    <t>PV_Device_Model_Info</t>
+  </si>
+  <si>
+    <t>PV_Firmware_Version</t>
+  </si>
+  <si>
+    <t>PV_DateTime</t>
+  </si>
+  <si>
+    <t>PV_Fault_1_0</t>
+  </si>
+  <si>
+    <t>PV_Fault_1_1</t>
+  </si>
+  <si>
+    <t>PV_Fault_1_2</t>
+  </si>
+  <si>
+    <t>PV_Fault_1_3</t>
+  </si>
+  <si>
+    <t>PV_Fault_1_4</t>
+  </si>
+  <si>
+    <t>PV_Fault_1_5</t>
+  </si>
+  <si>
+    <t>PV_Fault_1_6</t>
+  </si>
+  <si>
+    <t>PV_Fault_1_7</t>
+  </si>
+  <si>
+    <t>PV_Fault_1_8</t>
+  </si>
+  <si>
+    <t>PV_Fault_2_1</t>
+  </si>
+  <si>
+    <t>PV_Fault_2_2</t>
+  </si>
+  <si>
+    <t>PV_Fault_2_3</t>
+  </si>
+  <si>
+    <t>PV_Fault_2_4</t>
+  </si>
+  <si>
+    <t>PV_Fault_2_5</t>
+  </si>
+  <si>
+    <t>PV_Fault_2_6</t>
+  </si>
+  <si>
+    <t>PV_Fault_2_7</t>
+  </si>
+  <si>
+    <t>PV_Fault_3_0</t>
+  </si>
+  <si>
+    <t>PV_Fault_3_1</t>
+  </si>
+  <si>
+    <t>PV_Fault_3_2</t>
+  </si>
+  <si>
+    <t>PV_Fault_3_3</t>
+  </si>
+  <si>
+    <t>PV_Fault_3_4</t>
+  </si>
+  <si>
+    <t>PV_Fault_3_5</t>
+  </si>
+  <si>
+    <t>PV_Fault_3_6</t>
+  </si>
+  <si>
+    <t>PV_Fault_3_7</t>
+  </si>
+  <si>
+    <t>PV_Fault_3_8</t>
+  </si>
+  <si>
+    <t>PV_Fault_3_9</t>
+  </si>
+  <si>
+    <t>PV_Fault_3_10</t>
+  </si>
+  <si>
+    <t>PV_Fault_ARM_0</t>
+  </si>
+  <si>
+    <t>PV_Fault_ARM_1</t>
+  </si>
+  <si>
+    <t>PV_Fault_ARM_2</t>
+  </si>
+  <si>
+    <t>PV_Period_1_Enabled</t>
+  </si>
+  <si>
+    <t>PV_Period_2_Enabled</t>
+  </si>
+  <si>
+    <t>PV_Period_3_Enabled</t>
+  </si>
+  <si>
+    <t>PV_Period_4_Enabled</t>
+  </si>
+  <si>
+    <t>PV_Period_5_Enabled</t>
+  </si>
+  <si>
+    <t>PV_Period_6_Enabled</t>
+  </si>
+  <si>
+    <t>PV_Period_1_Start_H</t>
+  </si>
+  <si>
+    <t>PV_Period_2_Start_H</t>
+  </si>
+  <si>
+    <t>PV_Period_3_Start_H</t>
+  </si>
+  <si>
+    <t>PV_Period_4_Start_H</t>
+  </si>
+  <si>
+    <t>PV_Period_5_Start_H</t>
+  </si>
+  <si>
+    <t>PV_Period_6_Start_H</t>
+  </si>
+  <si>
+    <t>PV_Period_1_Start_M</t>
+  </si>
+  <si>
+    <t>PV_Period_2_Start_M</t>
+  </si>
+  <si>
+    <t>PV_Period_3_Start_M</t>
+  </si>
+  <si>
+    <t>PV_Period_4_Start_M</t>
+  </si>
+  <si>
+    <t>PV_Period_5_Start_M</t>
+  </si>
+  <si>
+    <t>PV_Period_6_Start_M</t>
+  </si>
+  <si>
+    <t>PV_Period_1_Stop_H</t>
+  </si>
+  <si>
+    <t>PV_Period_2_Stop_H</t>
+  </si>
+  <si>
+    <t>PV_Period_3_Stop_H</t>
+  </si>
+  <si>
+    <t>PV_Period_4_Stop_H</t>
+  </si>
+  <si>
+    <t>PV_Period_5_Stop_H</t>
+  </si>
+  <si>
+    <t>PV_Period_6_Stop_H</t>
+  </si>
+  <si>
+    <t>PV_Period_1_Stop_M</t>
+  </si>
+  <si>
+    <t>PV_Period_2_Stop_M</t>
+  </si>
+  <si>
+    <t>PV_Period_3_Stop_M</t>
+  </si>
+  <si>
+    <t>PV_Period_4_Stop_M</t>
+  </si>
+  <si>
+    <t>PV_Period_5_Stop_M</t>
+  </si>
+  <si>
+    <t>PV_Period_6_Stop_M</t>
+  </si>
+  <si>
+    <t>const MANUAL_DATA = [];</t>
+  </si>
+  <si>
+    <t>Period X</t>
+  </si>
+  <si>
+    <t>Period 1</t>
+  </si>
+  <si>
+    <t>Period 2</t>
+  </si>
+  <si>
+    <t>Period 3</t>
+  </si>
+  <si>
+    <t>Period 4</t>
+  </si>
+  <si>
+    <t>Period 5</t>
+  </si>
+  <si>
+    <t>Period 6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1124,6 +1344,24 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Cali "/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1176,7 +1414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1202,14 +1440,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1566,9 +1806,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q259"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q149" sqref="Q149:Q152"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q243" sqref="Q243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1951,7 +2191,7 @@
       <c r="I13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="J13" s="19" t="s">
         <v>27</v>
       </c>
       <c r="L13" s="16">
@@ -1992,7 +2232,7 @@
       <c r="I14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="18"/>
+      <c r="J14" s="19"/>
       <c r="L14" s="16">
         <v>1</v>
       </c>
@@ -2031,7 +2271,7 @@
       <c r="I15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="18"/>
+      <c r="J15" s="19"/>
       <c r="L15" s="16">
         <v>1</v>
       </c>
@@ -2152,7 +2392,7 @@
       <c r="I18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="18" t="s">
+      <c r="J18" s="19" t="s">
         <v>34</v>
       </c>
       <c r="L18" s="16">
@@ -2196,7 +2436,7 @@
       <c r="I19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J19" s="18"/>
+      <c r="J19" s="19"/>
       <c r="L19" s="16">
         <v>1</v>
       </c>
@@ -2232,7 +2472,7 @@
       <c r="I20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J20" s="18"/>
+      <c r="J20" s="19"/>
       <c r="L20" s="16">
         <v>1</v>
       </c>
@@ -2274,7 +2514,7 @@
       <c r="I21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J21" s="18"/>
+      <c r="J21" s="19"/>
       <c r="L21" s="16">
         <v>1</v>
       </c>
@@ -2310,7 +2550,7 @@
       <c r="I22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J22" s="18"/>
+      <c r="J22" s="19"/>
       <c r="L22" s="16">
         <v>1</v>
       </c>
@@ -2352,7 +2592,7 @@
       <c r="I23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J23" s="18"/>
+      <c r="J23" s="19"/>
       <c r="L23" s="16">
         <v>1</v>
       </c>
@@ -2388,7 +2628,7 @@
       <c r="I24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J24" s="18"/>
+      <c r="J24" s="19"/>
       <c r="P24" s="1" t="s">
         <v>310</v>
       </c>
@@ -3947,7 +4187,7 @@
       <c r="I68" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J68" s="18" t="s">
+      <c r="J68" s="19" t="s">
         <v>34</v>
       </c>
       <c r="L68" s="16">
@@ -3991,7 +4231,7 @@
       <c r="I69" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J69" s="18"/>
+      <c r="J69" s="19"/>
       <c r="L69" s="16">
         <v>1</v>
       </c>
@@ -6765,13 +7005,13 @@
       <c r="D149" s="1">
         <v>1</v>
       </c>
-      <c r="E149" s="19" t="s">
+      <c r="E149" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="F149" s="18" t="s">
+      <c r="F149" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="G149" s="18" t="s">
+      <c r="G149" s="19" t="s">
         <v>19</v>
       </c>
       <c r="H149" s="1" t="s">
@@ -6806,9 +7046,9 @@
       <c r="D150" s="1">
         <v>1</v>
       </c>
-      <c r="E150" s="19"/>
-      <c r="F150" s="18"/>
-      <c r="G150" s="18"/>
+      <c r="E150" s="20"/>
+      <c r="F150" s="19"/>
+      <c r="G150" s="19"/>
       <c r="H150" s="1" t="s">
         <v>15</v>
       </c>
@@ -6841,9 +7081,9 @@
       <c r="D151" s="1">
         <v>1</v>
       </c>
-      <c r="E151" s="19"/>
-      <c r="F151" s="18"/>
-      <c r="G151" s="18"/>
+      <c r="E151" s="20"/>
+      <c r="F151" s="19"/>
+      <c r="G151" s="19"/>
       <c r="H151" s="1" t="s">
         <v>15</v>
       </c>
@@ -8802,7 +9042,7 @@
         <v>306</v>
       </c>
       <c r="Q201" s="1" t="s">
-        <v>328</v>
+        <v>396</v>
       </c>
     </row>
     <row r="202" spans="1:17" ht="45" customHeight="1">
@@ -8840,7 +9080,7 @@
         <v>314</v>
       </c>
       <c r="Q202" s="1" t="s">
-        <v>328</v>
+        <v>397</v>
       </c>
     </row>
     <row r="203" spans="1:17" ht="30" customHeight="1">
@@ -8881,7 +9121,7 @@
         <v>310</v>
       </c>
       <c r="Q203" s="1" t="s">
-        <v>328</v>
+        <v>397</v>
       </c>
     </row>
     <row r="204" spans="1:17" ht="30" customHeight="1">
@@ -8922,7 +9162,7 @@
         <v>317</v>
       </c>
       <c r="Q204" s="1" t="s">
-        <v>328</v>
+        <v>397</v>
       </c>
     </row>
     <row r="205" spans="1:17" ht="30" customHeight="1">
@@ -8960,7 +9200,7 @@
         <v>310</v>
       </c>
       <c r="Q205" s="1" t="s">
-        <v>328</v>
+        <v>397</v>
       </c>
     </row>
     <row r="206" spans="1:17" ht="30" customHeight="1">
@@ -9001,7 +9241,7 @@
         <v>317</v>
       </c>
       <c r="Q206" s="1" t="s">
-        <v>328</v>
+        <v>397</v>
       </c>
     </row>
     <row r="207" spans="1:17">
@@ -9032,7 +9272,7 @@
       <c r="I207" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J207" s="17" t="s">
+      <c r="J207" s="21" t="s">
         <v>214</v>
       </c>
       <c r="L207" s="1">
@@ -9042,7 +9282,7 @@
         <v>311</v>
       </c>
       <c r="Q207" s="1" t="s">
-        <v>328</v>
+        <v>397</v>
       </c>
     </row>
     <row r="208" spans="1:17">
@@ -9073,7 +9313,7 @@
       <c r="I208" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J208" s="17"/>
+      <c r="J208" s="21"/>
       <c r="L208" s="1">
         <v>1</v>
       </c>
@@ -9081,7 +9321,7 @@
         <v>311</v>
       </c>
       <c r="Q208" s="1" t="s">
-        <v>328</v>
+        <v>397</v>
       </c>
     </row>
     <row r="209" spans="1:17">
@@ -9112,14 +9352,14 @@
       <c r="I209" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J209" s="17" t="s">
+      <c r="J209" s="21" t="s">
         <v>217</v>
       </c>
       <c r="P209" s="1" t="s">
         <v>314</v>
       </c>
       <c r="Q209" s="1" t="s">
-        <v>328</v>
+        <v>398</v>
       </c>
     </row>
     <row r="210" spans="1:17">
@@ -9150,7 +9390,7 @@
       <c r="I210" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J210" s="17"/>
+      <c r="J210" s="21"/>
       <c r="M210" s="1" t="s">
         <v>289</v>
       </c>
@@ -9158,7 +9398,7 @@
         <v>310</v>
       </c>
       <c r="Q210" s="1" t="s">
-        <v>328</v>
+        <v>398</v>
       </c>
     </row>
     <row r="211" spans="1:17">
@@ -9189,7 +9429,7 @@
       <c r="I211" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J211" s="17"/>
+      <c r="J211" s="21"/>
       <c r="O211" s="1">
         <v>1</v>
       </c>
@@ -9197,7 +9437,7 @@
         <v>317</v>
       </c>
       <c r="Q211" s="1" t="s">
-        <v>328</v>
+        <v>398</v>
       </c>
     </row>
     <row r="212" spans="1:17">
@@ -9228,12 +9468,12 @@
       <c r="I212" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J212" s="17"/>
+      <c r="J212" s="21"/>
       <c r="P212" s="1" t="s">
         <v>310</v>
       </c>
       <c r="Q212" s="1" t="s">
-        <v>328</v>
+        <v>398</v>
       </c>
     </row>
     <row r="213" spans="1:17">
@@ -9264,7 +9504,7 @@
       <c r="I213" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J213" s="17"/>
+      <c r="J213" s="21"/>
       <c r="O213" s="1">
         <v>1</v>
       </c>
@@ -9272,7 +9512,7 @@
         <v>317</v>
       </c>
       <c r="Q213" s="1" t="s">
-        <v>328</v>
+        <v>398</v>
       </c>
     </row>
     <row r="214" spans="1:17">
@@ -9303,7 +9543,7 @@
       <c r="I214" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J214" s="17"/>
+      <c r="J214" s="21"/>
       <c r="L214" s="1">
         <v>1</v>
       </c>
@@ -9311,7 +9551,7 @@
         <v>311</v>
       </c>
       <c r="Q214" s="1" t="s">
-        <v>328</v>
+        <v>398</v>
       </c>
     </row>
     <row r="215" spans="1:17">
@@ -9342,7 +9582,7 @@
       <c r="I215" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J215" s="17"/>
+      <c r="J215" s="21"/>
       <c r="L215" s="1">
         <v>1</v>
       </c>
@@ -9350,7 +9590,7 @@
         <v>311</v>
       </c>
       <c r="Q215" s="1" t="s">
-        <v>328</v>
+        <v>398</v>
       </c>
     </row>
     <row r="216" spans="1:17">
@@ -9381,14 +9621,14 @@
       <c r="I216" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J216" s="17" t="s">
+      <c r="J216" s="21" t="s">
         <v>218</v>
       </c>
       <c r="P216" s="1" t="s">
         <v>314</v>
       </c>
       <c r="Q216" s="1" t="s">
-        <v>328</v>
+        <v>399</v>
       </c>
     </row>
     <row r="217" spans="1:17">
@@ -9419,7 +9659,7 @@
       <c r="I217" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J217" s="17"/>
+      <c r="J217" s="21"/>
       <c r="M217" s="1" t="s">
         <v>289</v>
       </c>
@@ -9427,7 +9667,7 @@
         <v>310</v>
       </c>
       <c r="Q217" s="1" t="s">
-        <v>328</v>
+        <v>399</v>
       </c>
     </row>
     <row r="218" spans="1:17">
@@ -9458,7 +9698,7 @@
       <c r="I218" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J218" s="17"/>
+      <c r="J218" s="21"/>
       <c r="O218" s="1">
         <v>1</v>
       </c>
@@ -9466,7 +9706,7 @@
         <v>317</v>
       </c>
       <c r="Q218" s="1" t="s">
-        <v>328</v>
+        <v>399</v>
       </c>
     </row>
     <row r="219" spans="1:17">
@@ -9497,12 +9737,12 @@
       <c r="I219" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J219" s="17"/>
+      <c r="J219" s="21"/>
       <c r="P219" s="1" t="s">
         <v>310</v>
       </c>
       <c r="Q219" s="1" t="s">
-        <v>328</v>
+        <v>399</v>
       </c>
     </row>
     <row r="220" spans="1:17">
@@ -9533,7 +9773,7 @@
       <c r="I220" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J220" s="17"/>
+      <c r="J220" s="21"/>
       <c r="O220" s="1">
         <v>1</v>
       </c>
@@ -9541,7 +9781,7 @@
         <v>317</v>
       </c>
       <c r="Q220" s="1" t="s">
-        <v>328</v>
+        <v>399</v>
       </c>
     </row>
     <row r="221" spans="1:17">
@@ -9572,7 +9812,7 @@
       <c r="I221" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J221" s="17"/>
+      <c r="J221" s="21"/>
       <c r="L221" s="1">
         <v>1</v>
       </c>
@@ -9580,7 +9820,7 @@
         <v>311</v>
       </c>
       <c r="Q221" s="1" t="s">
-        <v>328</v>
+        <v>399</v>
       </c>
     </row>
     <row r="222" spans="1:17">
@@ -9611,7 +9851,7 @@
       <c r="I222" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J222" s="17"/>
+      <c r="J222" s="21"/>
       <c r="L222" s="1">
         <v>1</v>
       </c>
@@ -9619,7 +9859,7 @@
         <v>311</v>
       </c>
       <c r="Q222" s="1" t="s">
-        <v>328</v>
+        <v>399</v>
       </c>
     </row>
     <row r="223" spans="1:17">
@@ -9650,14 +9890,14 @@
       <c r="I223" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J223" s="17" t="s">
+      <c r="J223" s="21" t="s">
         <v>219</v>
       </c>
       <c r="P223" s="1" t="s">
         <v>314</v>
       </c>
       <c r="Q223" s="1" t="s">
-        <v>328</v>
+        <v>400</v>
       </c>
     </row>
     <row r="224" spans="1:17">
@@ -9688,7 +9928,7 @@
       <c r="I224" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J224" s="17"/>
+      <c r="J224" s="21"/>
       <c r="M224" s="1" t="s">
         <v>289</v>
       </c>
@@ -9696,7 +9936,7 @@
         <v>310</v>
       </c>
       <c r="Q224" s="1" t="s">
-        <v>328</v>
+        <v>400</v>
       </c>
     </row>
     <row r="225" spans="1:17">
@@ -9727,7 +9967,7 @@
       <c r="I225" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J225" s="17"/>
+      <c r="J225" s="21"/>
       <c r="O225" s="1">
         <v>1</v>
       </c>
@@ -9735,7 +9975,7 @@
         <v>317</v>
       </c>
       <c r="Q225" s="1" t="s">
-        <v>328</v>
+        <v>400</v>
       </c>
     </row>
     <row r="226" spans="1:17">
@@ -9766,12 +10006,12 @@
       <c r="I226" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J226" s="17"/>
+      <c r="J226" s="21"/>
       <c r="P226" s="1" t="s">
         <v>310</v>
       </c>
       <c r="Q226" s="1" t="s">
-        <v>328</v>
+        <v>400</v>
       </c>
     </row>
     <row r="227" spans="1:17">
@@ -9802,7 +10042,7 @@
       <c r="I227" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J227" s="17"/>
+      <c r="J227" s="21"/>
       <c r="O227" s="1">
         <v>1</v>
       </c>
@@ -9810,7 +10050,7 @@
         <v>317</v>
       </c>
       <c r="Q227" s="1" t="s">
-        <v>328</v>
+        <v>400</v>
       </c>
     </row>
     <row r="228" spans="1:17">
@@ -9841,7 +10081,7 @@
       <c r="I228" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J228" s="17"/>
+      <c r="J228" s="21"/>
       <c r="L228" s="1">
         <v>1</v>
       </c>
@@ -9849,7 +10089,7 @@
         <v>311</v>
       </c>
       <c r="Q228" s="1" t="s">
-        <v>328</v>
+        <v>400</v>
       </c>
     </row>
     <row r="229" spans="1:17">
@@ -9880,7 +10120,7 @@
       <c r="I229" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J229" s="17"/>
+      <c r="J229" s="21"/>
       <c r="L229" s="1">
         <v>1</v>
       </c>
@@ -9888,7 +10128,7 @@
         <v>311</v>
       </c>
       <c r="Q229" s="1" t="s">
-        <v>328</v>
+        <v>400</v>
       </c>
     </row>
     <row r="230" spans="1:17">
@@ -9919,14 +10159,14 @@
       <c r="I230" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J230" s="17" t="s">
+      <c r="J230" s="21" t="s">
         <v>220</v>
       </c>
       <c r="P230" s="1" t="s">
         <v>314</v>
       </c>
       <c r="Q230" s="1" t="s">
-        <v>328</v>
+        <v>401</v>
       </c>
     </row>
     <row r="231" spans="1:17">
@@ -9957,7 +10197,7 @@
       <c r="I231" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J231" s="17"/>
+      <c r="J231" s="21"/>
       <c r="M231" s="1" t="s">
         <v>289</v>
       </c>
@@ -9965,7 +10205,7 @@
         <v>310</v>
       </c>
       <c r="Q231" s="1" t="s">
-        <v>328</v>
+        <v>401</v>
       </c>
     </row>
     <row r="232" spans="1:17">
@@ -9996,7 +10236,7 @@
       <c r="I232" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J232" s="17"/>
+      <c r="J232" s="21"/>
       <c r="O232" s="1">
         <v>1</v>
       </c>
@@ -10004,7 +10244,7 @@
         <v>317</v>
       </c>
       <c r="Q232" s="1" t="s">
-        <v>328</v>
+        <v>401</v>
       </c>
     </row>
     <row r="233" spans="1:17">
@@ -10035,12 +10275,12 @@
       <c r="I233" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J233" s="17"/>
+      <c r="J233" s="21"/>
       <c r="P233" s="1" t="s">
         <v>310</v>
       </c>
       <c r="Q233" s="1" t="s">
-        <v>328</v>
+        <v>401</v>
       </c>
     </row>
     <row r="234" spans="1:17">
@@ -10071,7 +10311,7 @@
       <c r="I234" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J234" s="17"/>
+      <c r="J234" s="21"/>
       <c r="O234" s="1">
         <v>1</v>
       </c>
@@ -10079,7 +10319,7 @@
         <v>317</v>
       </c>
       <c r="Q234" s="1" t="s">
-        <v>328</v>
+        <v>401</v>
       </c>
     </row>
     <row r="235" spans="1:17">
@@ -10110,7 +10350,7 @@
       <c r="I235" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J235" s="17"/>
+      <c r="J235" s="21"/>
       <c r="L235" s="1">
         <v>1</v>
       </c>
@@ -10118,7 +10358,7 @@
         <v>311</v>
       </c>
       <c r="Q235" s="1" t="s">
-        <v>328</v>
+        <v>401</v>
       </c>
     </row>
     <row r="236" spans="1:17">
@@ -10149,7 +10389,7 @@
       <c r="I236" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J236" s="17"/>
+      <c r="J236" s="21"/>
       <c r="L236" s="1">
         <v>1</v>
       </c>
@@ -10157,7 +10397,7 @@
         <v>311</v>
       </c>
       <c r="Q236" s="1" t="s">
-        <v>328</v>
+        <v>401</v>
       </c>
     </row>
     <row r="237" spans="1:17">
@@ -10188,14 +10428,14 @@
       <c r="I237" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J237" s="17" t="s">
+      <c r="J237" s="21" t="s">
         <v>221</v>
       </c>
       <c r="P237" s="1" t="s">
         <v>314</v>
       </c>
       <c r="Q237" s="1" t="s">
-        <v>328</v>
+        <v>402</v>
       </c>
     </row>
     <row r="238" spans="1:17">
@@ -10226,7 +10466,7 @@
       <c r="I238" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J238" s="17"/>
+      <c r="J238" s="21"/>
       <c r="M238" s="1" t="s">
         <v>289</v>
       </c>
@@ -10234,7 +10474,7 @@
         <v>310</v>
       </c>
       <c r="Q238" s="1" t="s">
-        <v>328</v>
+        <v>402</v>
       </c>
     </row>
     <row r="239" spans="1:17">
@@ -10265,7 +10505,7 @@
       <c r="I239" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J239" s="17"/>
+      <c r="J239" s="21"/>
       <c r="O239" s="1">
         <v>1</v>
       </c>
@@ -10273,7 +10513,7 @@
         <v>317</v>
       </c>
       <c r="Q239" s="1" t="s">
-        <v>328</v>
+        <v>402</v>
       </c>
     </row>
     <row r="240" spans="1:17">
@@ -10304,12 +10544,12 @@
       <c r="I240" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J240" s="17"/>
+      <c r="J240" s="21"/>
       <c r="P240" s="1" t="s">
         <v>310</v>
       </c>
       <c r="Q240" s="1" t="s">
-        <v>328</v>
+        <v>402</v>
       </c>
     </row>
     <row r="241" spans="1:17">
@@ -10340,7 +10580,7 @@
       <c r="I241" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J241" s="17"/>
+      <c r="J241" s="21"/>
       <c r="O241" s="1">
         <v>1</v>
       </c>
@@ -10348,7 +10588,7 @@
         <v>317</v>
       </c>
       <c r="Q241" s="1" t="s">
-        <v>328</v>
+        <v>402</v>
       </c>
     </row>
     <row r="242" spans="1:17">
@@ -10379,7 +10619,7 @@
       <c r="I242" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J242" s="17"/>
+      <c r="J242" s="21"/>
       <c r="L242" s="1">
         <v>1</v>
       </c>
@@ -10387,7 +10627,7 @@
         <v>311</v>
       </c>
       <c r="Q242" s="1" t="s">
-        <v>328</v>
+        <v>402</v>
       </c>
     </row>
     <row r="243" spans="1:17">
@@ -10418,7 +10658,7 @@
       <c r="I243" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J243" s="17"/>
+      <c r="J243" s="21"/>
       <c r="L243" s="1">
         <v>1</v>
       </c>
@@ -10426,7 +10666,7 @@
         <v>311</v>
       </c>
       <c r="Q243" s="1" t="s">
-        <v>328</v>
+        <v>402</v>
       </c>
     </row>
     <row r="244" spans="1:17">
@@ -10539,7 +10779,7 @@
       <c r="I246" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J246" s="17" t="s">
+      <c r="J246" s="21" t="s">
         <v>226</v>
       </c>
       <c r="O246" s="1">
@@ -10580,7 +10820,7 @@
       <c r="I247" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J247" s="17"/>
+      <c r="J247" s="21"/>
       <c r="O247" s="1">
         <v>1</v>
       </c>
@@ -10619,7 +10859,7 @@
       <c r="I248" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J248" s="17"/>
+      <c r="J248" s="21"/>
       <c r="O248" s="1">
         <v>1</v>
       </c>
@@ -10658,7 +10898,7 @@
       <c r="I249" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J249" s="18" t="s">
+      <c r="J249" s="19" t="s">
         <v>223</v>
       </c>
       <c r="O249" s="1">
@@ -10699,7 +10939,7 @@
       <c r="I250" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J250" s="18"/>
+      <c r="J250" s="19"/>
       <c r="O250" s="1">
         <v>1</v>
       </c>
@@ -10738,7 +10978,7 @@
       <c r="I251" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J251" s="18" t="s">
+      <c r="J251" s="19" t="s">
         <v>223</v>
       </c>
       <c r="O251" s="1">
@@ -10779,7 +11019,7 @@
       <c r="I252" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J252" s="18"/>
+      <c r="J252" s="19"/>
       <c r="O252" s="1">
         <v>1</v>
       </c>
@@ -10818,7 +11058,7 @@
       <c r="I253" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J253" s="18"/>
+      <c r="J253" s="19"/>
       <c r="O253" s="1">
         <v>1</v>
       </c>
@@ -10857,7 +11097,7 @@
       <c r="I254" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J254" s="18"/>
+      <c r="J254" s="19"/>
       <c r="O254" s="1">
         <v>1</v>
       </c>
@@ -10896,7 +11136,7 @@
       <c r="I255" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J255" s="18"/>
+      <c r="J255" s="19"/>
       <c r="O255" s="1">
         <v>1</v>
       </c>
@@ -10935,7 +11175,7 @@
       <c r="I256" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J256" s="18"/>
+      <c r="J256" s="19"/>
       <c r="O256" s="1">
         <v>1</v>
       </c>
@@ -10974,7 +11214,7 @@
       <c r="I257" s="1">
         <v>10</v>
       </c>
-      <c r="J257" s="18"/>
+      <c r="J257" s="19"/>
       <c r="O257" s="1">
         <v>1</v>
       </c>
@@ -11070,12 +11310,6 @@
   </sheetData>
   <autoFilter ref="A1:Q259" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="15">
-    <mergeCell ref="J13:J15"/>
-    <mergeCell ref="J18:J24"/>
-    <mergeCell ref="J68:J69"/>
-    <mergeCell ref="E149:E151"/>
-    <mergeCell ref="F149:F151"/>
-    <mergeCell ref="G149:G151"/>
     <mergeCell ref="J237:J243"/>
     <mergeCell ref="J246:J248"/>
     <mergeCell ref="J249:J250"/>
@@ -11085,6 +11319,12 @@
     <mergeCell ref="J216:J222"/>
     <mergeCell ref="J223:J229"/>
     <mergeCell ref="J230:J236"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="J18:J24"/>
+    <mergeCell ref="J68:J69"/>
+    <mergeCell ref="E149:E151"/>
+    <mergeCell ref="F149:F151"/>
+    <mergeCell ref="G149:G151"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="0"/>
@@ -11781,4 +12021,807 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A145AA7-9EA1-42EE-A176-4D22B50CD094}">
+  <dimension ref="A1:D65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="11.42578125" style="17"/>
+    <col min="5" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="18" t="str">
+        <f>"MANUAL_DATA.push({item: '"&amp;A2&amp;"', sitemap: '"&amp;B2&amp;"'});"</f>
+        <v>MANUAL_DATA.push({item: 'PV_Device_SN', sitemap: 'Infos'});</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D3" s="18" t="str">
+        <f t="shared" ref="D3:D65" si="0">"MANUAL_DATA.push({item: '"&amp;A3&amp;"', sitemap: '"&amp;B3&amp;"'});"</f>
+        <v>MANUAL_DATA.push({item: 'PV_Device_Model_Info', sitemap: 'Infos'});</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D4" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Firmware_Version', sitemap: 'Infos'});</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D5" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_DateTime', sitemap: 'Infos'});</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D6" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_1_0', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D7" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_1_1', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D8" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_1_2', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D9" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_1_3', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D10" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_1_4', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D11" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_1_5', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D12" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_1_6', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D13" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_1_7', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D14" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_1_8', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D15" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_2_1', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D16" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_2_2', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D17" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_2_3', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D18" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_2_4', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D19" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_2_5', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D20" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_2_6', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D21" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_2_7', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D22" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_3_0', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D23" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_3_1', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D24" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_3_2', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D25" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_3_3', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D26" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_3_4', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D27" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_3_5', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D28" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_3_6', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D29" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_3_7', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D30" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_3_8', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D31" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_3_9', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D32" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_3_10', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D33" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_ARM_0', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D34" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_ARM_1', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D35" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Fault_ARM_2', sitemap: 'Status'});</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D36" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_1_Enabled', sitemap: 'Period 1'});</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D37" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_2_Enabled', sitemap: 'Period 2'});</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D38" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_3_Enabled', sitemap: 'Period 3'});</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D39" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_4_Enabled', sitemap: 'Period 4'});</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D40" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_5_Enabled', sitemap: 'Period 5'});</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D41" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_6_Enabled', sitemap: 'Period 6'});</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D42" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_1_Start_H', sitemap: 'Period 1'});</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D43" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_2_Start_H', sitemap: 'Period 2'});</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D44" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_3_Start_H', sitemap: 'Period 3'});</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D45" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_4_Start_H', sitemap: 'Period 4'});</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D46" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_5_Start_H', sitemap: 'Period 5'});</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D47" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_6_Start_H', sitemap: 'Period 6'});</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D48" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_1_Start_M', sitemap: 'Period 1'});</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D49" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_2_Start_M', sitemap: 'Period 2'});</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D50" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_3_Start_M', sitemap: 'Period 3'});</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D51" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_4_Start_M', sitemap: 'Period 4'});</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D52" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_5_Start_M', sitemap: 'Period 5'});</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D53" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_6_Start_M', sitemap: 'Period 6'});</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D54" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_1_Stop_H', sitemap: 'Period 1'});</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D55" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_2_Stop_H', sitemap: 'Period 2'});</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D56" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_3_Stop_H', sitemap: 'Period 3'});</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D57" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_4_Stop_H', sitemap: 'Period 4'});</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D58" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_5_Stop_H', sitemap: 'Period 5'});</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D59" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_6_Stop_H', sitemap: 'Period 6'});</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D60" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_1_Stop_M', sitemap: 'Period 1'});</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D61" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_2_Stop_M', sitemap: 'Period 2'});</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D62" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_3_Stop_M', sitemap: 'Period 3'});</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D63" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_4_Stop_M', sitemap: 'Period 4'});</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D64" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_5_Stop_M', sitemap: 'Period 5'});</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D65" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>MANUAL_DATA.push({item: 'PV_Period_6_Stop_M', sitemap: 'Period 6'});</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>